<commit_message>
added Procfile, dropbox connection, updated script for data fetching and uploading
</commit_message>
<xml_diff>
--- a/output/crypto_analysis.xlsx
+++ b/output/crypto_analysis.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>market_cap</t>
         </is>
       </c>
@@ -454,8 +459,13 @@
           <t>Bitcoin</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1934371283796.188</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BTC</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1872066201124.301</v>
       </c>
     </row>
     <row r="3">
@@ -464,8 +474,13 @@
           <t>Ethereum</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>416637876917.9184</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>398474056364.7794</v>
       </c>
     </row>
     <row r="4">
@@ -474,8 +489,13 @@
           <t>Tether USDt</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>137517986711.4266</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>137556493146.6945</v>
       </c>
     </row>
     <row r="5">
@@ -484,8 +504,13 @@
           <t>XRP</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>132818042883.7128</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>133204662185.7822</v>
       </c>
     </row>
     <row r="6">
@@ -494,8 +519,20 @@
           <t>BNB</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>102241375252.4961</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BNB</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>99835401046.23409</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Last updated (GMT): 2025-01-09 00:07:13</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -509,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +563,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2078.232201716744</v>
+        <v>2009.267132097337</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Last updated (GMT): 2025-01-09 00:07:13</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -556,18 +598,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>percent_change_24h</t>
+          <t>change</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bitget Token</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>3.2722597</v>
+          <t>MANTRA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Last updated (GMT): 2025-01-09 00:07:13</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -597,18 +641,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>percent_change_24h</t>
+          <t>change</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VeChain</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-10.52395395</v>
+          <t>Ethena</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Last updated (GMT): 2025-01-09 00:07:13</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>